<commit_message>
Changes for Excel Reports
</commit_message>
<xml_diff>
--- a/NtierMvc/App_Data/Documents/Excel/EnquiryandQutoeRegister.xlsx
+++ b/NtierMvc/App_Data/Documents/Excel/EnquiryandQutoeRegister.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Downloads\C#\NtierMvc\App_Data\Documents\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890CD1EF-1453-4AF2-AEC3-E632F5367B18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19800" windowHeight="7665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -181,13 +187,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00\ ;\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="167" formatCode="0_);\(0\)"/>
-    <numFmt numFmtId="168" formatCode="#.00"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00;[Red]&quot;-&quot;#,##0.00"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00\ ;\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0_);\(0\)"/>
+    <numFmt numFmtId="166" formatCode="#.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00;[Red]&quot;-&quot;#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -754,7 +760,7 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -767,7 +773,7 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="0">
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
@@ -781,7 +787,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="38" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -801,8 +807,8 @@
     <xf numFmtId="10" fontId="12" fillId="7" borderId="9" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -815,7 +821,7 @@
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1">
@@ -869,24 +875,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="9" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -896,24 +884,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -944,27 +917,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="9" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -974,63 +947,87 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="55">
-    <cellStyle name="Accent1 - 20%" xfId="5"/>
-    <cellStyle name="Accent1 - 40%" xfId="13"/>
-    <cellStyle name="Accent1 - 60%" xfId="2"/>
-    <cellStyle name="Accent2 - 20%" xfId="12"/>
-    <cellStyle name="Accent2 - 40%" xfId="1"/>
-    <cellStyle name="Accent2 - 60%" xfId="14"/>
-    <cellStyle name="Accent3 - 20%" xfId="15"/>
-    <cellStyle name="Accent3 - 40%" xfId="7"/>
-    <cellStyle name="Accent3 - 60%" xfId="9"/>
-    <cellStyle name="Accent4 - 20%" xfId="16"/>
-    <cellStyle name="Accent4 - 40%" xfId="4"/>
-    <cellStyle name="Accent4 - 60%" xfId="17"/>
-    <cellStyle name="Accent5 - 20%" xfId="3"/>
-    <cellStyle name="Accent5 - 40%" xfId="18"/>
-    <cellStyle name="Accent5 - 60%" xfId="11"/>
-    <cellStyle name="Accent6 - 20%" xfId="19"/>
-    <cellStyle name="Accent6 - 40%" xfId="20"/>
-    <cellStyle name="Accent6 - 60%" xfId="21"/>
-    <cellStyle name="Cabecera 1" xfId="6"/>
-    <cellStyle name="Cabecera 2" xfId="8"/>
-    <cellStyle name="category" xfId="22"/>
-    <cellStyle name="Currency $" xfId="23"/>
-    <cellStyle name="Date" xfId="24"/>
-    <cellStyle name="Emphasis 1" xfId="25"/>
-    <cellStyle name="Emphasis 2" xfId="26"/>
-    <cellStyle name="Emphasis 3" xfId="27"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="28"/>
-    <cellStyle name="Excel Built-in Normal" xfId="29"/>
-    <cellStyle name="Fecha" xfId="30"/>
-    <cellStyle name="Fijo" xfId="32"/>
-    <cellStyle name="Fixed" xfId="33"/>
-    <cellStyle name="Grey" xfId="34"/>
-    <cellStyle name="HEADER" xfId="35"/>
-    <cellStyle name="Heading1" xfId="36"/>
-    <cellStyle name="Heading2" xfId="37"/>
-    <cellStyle name="Hyperlink 3" xfId="38"/>
-    <cellStyle name="Input [yellow]" xfId="39"/>
-    <cellStyle name="Millares_DIM" xfId="40"/>
-    <cellStyle name="Model" xfId="41"/>
-    <cellStyle name="Moneda_DIM" xfId="42"/>
-    <cellStyle name="Monetario0" xfId="43"/>
+    <cellStyle name="Accent1 - 20%" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent1 - 40%" xfId="13" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent1 - 60%" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent2 - 20%" xfId="12" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Accent2 - 40%" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Accent2 - 60%" xfId="14" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Accent3 - 20%" xfId="15" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Accent3 - 40%" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Accent3 - 60%" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Accent4 - 20%" xfId="16" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Accent4 - 40%" xfId="4" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Accent4 - 60%" xfId="17" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Accent5 - 20%" xfId="3" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Accent5 - 40%" xfId="18" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Accent5 - 60%" xfId="11" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Accent6 - 20%" xfId="19" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Accent6 - 40%" xfId="20" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Accent6 - 60%" xfId="21" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Cabecera 1" xfId="6" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Cabecera 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="category" xfId="22" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Currency $" xfId="23" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Date" xfId="24" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Emphasis 1" xfId="25" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Emphasis 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Emphasis 3" xfId="27" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="28" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="29" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Fecha" xfId="30" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Fijo" xfId="32" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Fixed" xfId="33" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Grey" xfId="34" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="HEADER" xfId="35" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Heading1" xfId="36" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Heading2" xfId="37" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Hyperlink 3" xfId="38" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Input [yellow]" xfId="39" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Millares_DIM" xfId="40" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Model" xfId="41" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Moneda_DIM" xfId="42" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Monetario0" xfId="43" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal - Style1" xfId="10"/>
-    <cellStyle name="Normal 10" xfId="44"/>
-    <cellStyle name="Normal 2" xfId="45"/>
-    <cellStyle name="Normal 3" xfId="46"/>
-    <cellStyle name="Normal 4" xfId="47"/>
-    <cellStyle name="Œ…‹æØ‚è [0.00]_PRODUCT DETAIL Q1" xfId="48"/>
-    <cellStyle name="Œ…‹æØ‚è_PRODUCT DETAIL Q1" xfId="49"/>
-    <cellStyle name="Percent [2]" xfId="50"/>
-    <cellStyle name="Percent 2" xfId="51"/>
-    <cellStyle name="Porcentual_DIM" xfId="52"/>
-    <cellStyle name="Punto0" xfId="53"/>
-    <cellStyle name="Sheet Title" xfId="31"/>
-    <cellStyle name="subhead" xfId="54"/>
+    <cellStyle name="Normal - Style1" xfId="10" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 10" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal 3" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Normal 4" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Œ…‹æØ‚è [0.00]_PRODUCT DETAIL Q1" xfId="48" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Œ…‹æØ‚è_PRODUCT DETAIL Q1" xfId="49" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Percent [2]" xfId="50" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Percent 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Porcentual_DIM" xfId="52" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Punto0" xfId="53" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Sheet Title" xfId="31" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="subhead" xfId="54" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1042,6 +1039,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1064,7 +1064,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="NEW MOT LOGO 11"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="NEW MOT LOGO 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1237,7 +1243,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1270,9 +1276,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1305,6 +1328,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1480,10 +1520,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleSheetLayoutView="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E6" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
@@ -1542,7 +1584,7 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
-      <c r="N2" s="40"/>
+      <c r="N2" s="29"/>
     </row>
     <row r="3" spans="1:14" ht="27.75" customHeight="1">
       <c r="A3" s="10"/>
@@ -1560,25 +1602,25 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
-      <c r="N3" s="41"/>
+      <c r="N3" s="30"/>
     </row>
     <row r="4" spans="1:14" ht="27.75" customHeight="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="53"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="42"/>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" ht="48" customHeight="1">
       <c r="A5" s="15" t="s">
@@ -1620,7 +1662,7 @@
       <c r="M5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="43" t="s">
+      <c r="N5" s="32" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1638,123 +1680,123 @@
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
       <c r="M6" s="16"/>
-      <c r="N6" s="43"/>
+      <c r="N6" s="32"/>
     </row>
     <row r="7" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="46"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="39"/>
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="47"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="45"/>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
       <c r="N9" s="48"/>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
       <c r="N10" s="48"/>
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
       <c r="N11" s="48"/>
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="32">
+      <c r="B12" s="20"/>
+      <c r="C12" s="22">
         <v>1</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="49"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="50"/>
     </row>
     <row r="13" spans="1:14" ht="41.25" customHeight="1">
       <c r="A13" s="13" t="s">
@@ -1765,8 +1807,8 @@
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="35" t="s">
+      <c r="G13" s="23"/>
+      <c r="H13" s="24" t="s">
         <v>28</v>
       </c>
       <c r="I13" s="14"/>
@@ -1774,7 +1816,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
-      <c r="N13" s="42"/>
+      <c r="N13" s="31"/>
     </row>
     <row r="14" spans="1:14" ht="49.5" customHeight="1">
       <c r="A14" s="13" t="s">
@@ -1785,8 +1827,8 @@
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35" t="s">
+      <c r="G14" s="23"/>
+      <c r="H14" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I14" s="14"/>
@@ -1794,27 +1836,27 @@
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
-      <c r="N14" s="42"/>
+      <c r="N14" s="31"/>
     </row>
     <row r="15" spans="1:14" ht="32.25" customHeight="1">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="39" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="50"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1822,8 +1864,8 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="69" fitToHeight="6" orientation="landscape"/>
+  <pageSetup paperSize="9" scale="69" fitToHeight="6" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>